<commit_message>
Added User needs and UI info
</commit_message>
<xml_diff>
--- a/Deliverable2/Docs/ExpectedBehavior.xlsx
+++ b/Deliverable2/Docs/ExpectedBehavior.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Baba\Georgia Tech\CS-6400-O01\github\RockStars\Deliverable2\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39000" yWindow="-120" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="39000" yWindow="-120" windowWidth="25605" windowHeight="17535" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="UI" sheetId="1" r:id="rId1"/>
+    <sheet name="Needs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Event</t>
   </si>
@@ -30,19 +36,107 @@
     <t>Expected Behavior</t>
   </si>
   <si>
-    <t>1. User selects a country from dropdown menu
-2. User clicks Recommended Vaccines icon</t>
-  </si>
-  <si>
-    <t>1. Name of country appears on the screen
-2. A list of recommended vaccines pops up</t>
+    <t>User Needs</t>
+  </si>
+  <si>
+    <t>Passive</t>
+  </si>
+  <si>
+    <t>List of Vaccines</t>
+  </si>
+  <si>
+    <t>Recommended off the shelf medicines</t>
+  </si>
+  <si>
+    <t>Tips to Prevent infections</t>
+  </si>
+  <si>
+    <t>Tips for self treatment incase of infections</t>
+  </si>
+  <si>
+    <t>Real Time</t>
+  </si>
+  <si>
+    <t>Location based Push Notification for outbreaks</t>
+  </si>
+  <si>
+    <t>User selects destination country from dropdown menu</t>
+  </si>
+  <si>
+    <t>Name of country appears on the screen</t>
+  </si>
+  <si>
+    <t>User clicks Recommended Vaccines icon</t>
+  </si>
+  <si>
+    <t>A list of recommended vaccines pops up</t>
+  </si>
+  <si>
+    <t>User clicks Packing List icon</t>
+  </si>
+  <si>
+    <t>Met</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>A list of recommended items to pack pops up</t>
+  </si>
+  <si>
+    <t>User receives list of outbreaks in local area via email</t>
+  </si>
+  <si>
+    <t>User clicks email notification icon</t>
+  </si>
+  <si>
+    <t>User clicks User Profile icon</t>
+  </si>
+  <si>
+    <t>A list of text boxes shows up ( Name, Age, Sex, Date of Birth,contact email and Submit button)</t>
+  </si>
+  <si>
+    <t>User clicks on Submit Button</t>
+  </si>
+  <si>
+    <t>A confirmation message showing "Thank You for submitting your information" pops up</t>
+  </si>
+  <si>
+    <t>User clicks Reset Button</t>
+  </si>
+  <si>
+    <t>The page goes to default state</t>
+  </si>
+  <si>
+    <t>User selects approximate date of travel to country from date menu</t>
+  </si>
+  <si>
+    <t>Date as selected by user appears on screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User enters address of SafeTravels website </t>
+  </si>
+  <si>
+    <t>SafeTravels website shows up on browser</t>
+  </si>
+  <si>
+    <t>User enters login information ( username, password)</t>
+  </si>
+  <si>
+    <t>If authenticated, the SafeTravels App screen shows up, otherwise message "incorrect login information" pops up</t>
+  </si>
+  <si>
+    <t>User clicks Exit Button</t>
+  </si>
+  <si>
+    <t>The page exits and login screen appears on the browser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -74,8 +168,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -88,8 +190,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -110,6 +218,139 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -134,15 +375,50 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -169,6 +445,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -494,47 +778,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="B2:C2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.375" customWidth="1"/>
+    <col min="3" max="3" width="21.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="75">
-      <c r="A2" s="3">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>